<commit_message>
modified:   dsyg_erp/WebRoot/page/warehouserpt/updwarehouserptout.jsp 	modified:   dsyg_erp/WebRoot/page/warehouserpt/updwarehouserptoutitem.jsp 	modified:   dsyg_erp/WebRoot/page/warehouserpt_out_detail_noprice_template.xlsx 	modified:   dsyg_erp/src/com/cn/common/factory/MatrixImageFactory.java 	modified:   dsyg_erp/src/com/cn/common/factory/Poi2007Base.java 	modified:   dsyg_erp/src/com/cn/common/factory/PoiFactory.java 	modified:   dsyg_erp/src/com/cn/common/factory/PoiWarehouserptOutDetail2.java 	modified:   dsyg_erp/src/com/cn/common/util/Constants.java 	modified:   dsyg_erp/src/com/cn/dsyg/action/WarehouserptAction.java 	modified:   dsyg_erp/src/com/cn/dsyg/service/impl/WarehouserptServiceImpl.java
</commit_message>
<xml_diff>
--- a/dsyg_erp/WebRoot/page/warehouserpt_out_detail_noprice_template.xlsx
+++ b/dsyg_erp/WebRoot/page/warehouserpt_out_detail_noprice_template.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="270" yWindow="585" windowWidth="19095" windowHeight="8325"/>
   </bookViews>
   <sheets>
-    <sheet name="sample" sheetId="1" r:id="rId1"/>
+    <sheet name="form" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>单位</t>
   </si>
@@ -22,15 +22,7 @@
     <t>数量</t>
   </si>
   <si>
-    <t>传真：</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>序号</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>业务员：</t>
     <phoneticPr fontId="4"/>
   </si>
   <si>
@@ -217,32 +209,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <r>
-      <t>送</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>货</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>地址2：</t>
-    </r>
-  </si>
-  <si>
     <t>电话：</t>
     <phoneticPr fontId="4"/>
   </si>
@@ -347,13 +313,39 @@
       <t>货单</t>
     </r>
     <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <r>
+      <t>送</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>货</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>地址2：</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -493,6 +485,11 @@
       <name val="SimSun-ExtB"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -583,7 +580,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -607,26 +604,9 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -641,10 +621,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -657,13 +633,38 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="21" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -970,7 +971,7 @@
   <dimension ref="A2:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -978,137 +979,133 @@
     <col min="1" max="2" width="5" customWidth="1"/>
     <col min="3" max="4" width="12.75" customWidth="1"/>
     <col min="5" max="5" width="14.875" customWidth="1"/>
-    <col min="6" max="6" width="12.75" customWidth="1"/>
-    <col min="7" max="7" width="6.375" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="14.25" customWidth="1"/>
+    <col min="6" max="6" width="11.875" customWidth="1"/>
+    <col min="7" max="7" width="5.25" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="21.875" customWidth="1"/>
     <col min="10" max="10" width="14.625" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
     <col min="12" max="12" width="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="26.25">
-      <c r="A2" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
+      <c r="A2" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
     </row>
     <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="6"/>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="6"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="26"/>
+      <c r="G4" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="17"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="6"/>
       <c r="B5" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" s="6"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="6"/>
       <c r="G5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="16"/>
-      <c r="L5" s="10"/>
+        <v>15</v>
+      </c>
+      <c r="I5" s="25"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="31"/>
     </row>
     <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="23"/>
+        <v>16</v>
+      </c>
+      <c r="I6" s="27"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="16"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="11"/>
+        <v>17</v>
+      </c>
+      <c r="I7" s="20"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="6"/>
       <c r="B8" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" s="6"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="I8" s="21"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="6"/>
       <c r="B9" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" s="6"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="16"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="23"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="I9" s="21"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="6"/>
       <c r="B10" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C10" s="6"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="16"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="23"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="13"/>
+      <c r="G10" s="7"/>
+      <c r="I10" s="33"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
     </row>
@@ -1120,9 +1117,9 @@
       <c r="E11" s="6"/>
       <c r="F11" s="2"/>
       <c r="G11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="24"/>
+        <v>18</v>
+      </c>
+      <c r="I11" s="32"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
     </row>
@@ -1131,34 +1128,34 @@
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="20"/>
-      <c r="F13" t="s">
-        <v>17</v>
+      <c r="A13" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="13"/>
+      <c r="F13" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" s="11" t="s">
         <v>5</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="9" t="s">
-        <v>7</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="1" t="s">
@@ -1168,7 +1165,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>